<commit_message>
Update S2B Data: 2025-11-25
</commit_message>
<xml_diff>
--- a/s2b_result.xlsx
+++ b/s2b_result.xlsx
@@ -436,14 +436,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>데이터없음</t>
+          <t>메시지 없음</t>
         </is>
       </c>
     </row>

</xml_diff>